<commit_message>
Importer: prevent product to be linked to variation child
Fix the product importer to prevent parent sku being the
current product or other variation child
</commit_message>
<xml_diff>
--- a/shuup_tests/importer/data/product/product_sample_import_with_variations.xlsx
+++ b/shuup_tests/importer/data/product/product_sample_import_with_variations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/panutulimaki/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31259E3-73F1-8B42-8A83-9E6CE41298E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223176F4-9DD5-BB49-A045-CCCA5123CA3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="46680" yWindow="460" windowWidth="43100" windowHeight="27620" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="43940" yWindow="460" windowWidth="43100" windowHeight="27620" tabRatio="993" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Taul1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="56">
   <si>
     <t>Ignore</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>This variation has faulty variation value</t>
+  </si>
+  <si>
+    <t>This tries to link variation to child</t>
   </si>
 </sst>
 </file>
@@ -629,10 +632,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N50"/>
+  <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I53" sqref="I52:I53"/>
+      <selection activeCell="B52" sqref="B52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2248,7 +2251,10 @@
         <v>42</v>
       </c>
       <c r="C46">
-        <v>22</v>
+        <v>28</v>
+      </c>
+      <c r="D46" t="s">
+        <v>55</v>
       </c>
       <c r="F46" t="s">
         <v>27</v>
@@ -2256,11 +2262,8 @@
       <c r="G46" t="s">
         <v>26</v>
       </c>
-      <c r="H46" t="s">
-        <v>41</v>
-      </c>
       <c r="I46">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="J46">
         <v>100</v>
@@ -2283,16 +2286,13 @@
         <v>42</v>
       </c>
       <c r="C47">
-        <v>1000</v>
-      </c>
-      <c r="D47" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="F47" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="G47" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="H47" t="s">
         <v>41</v>
@@ -2301,7 +2301,7 @@
         <v>10</v>
       </c>
       <c r="J47">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="K47" t="s">
         <v>16</v>
@@ -2321,10 +2321,10 @@
         <v>42</v>
       </c>
       <c r="C48">
-        <v>31</v>
+        <v>1000</v>
       </c>
       <c r="D48" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="F48" t="s">
         <v>49</v>
@@ -2359,16 +2359,16 @@
         <v>42</v>
       </c>
       <c r="C49">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D49" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F49" t="s">
         <v>49</v>
       </c>
       <c r="G49" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H49" t="s">
         <v>41</v>
@@ -2406,7 +2406,7 @@
         <v>49</v>
       </c>
       <c r="G50" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H50" t="s">
         <v>41</v>
@@ -2427,6 +2427,44 @@
         <v>18</v>
       </c>
       <c r="N50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51">
+        <v>42</v>
+      </c>
+      <c r="C51">
+        <v>22</v>
+      </c>
+      <c r="D51" t="s">
+        <v>54</v>
+      </c>
+      <c r="F51" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+      <c r="H51" t="s">
+        <v>41</v>
+      </c>
+      <c r="I51">
+        <v>10</v>
+      </c>
+      <c r="J51">
+        <v>101</v>
+      </c>
+      <c r="K51" t="s">
+        <v>16</v>
+      </c>
+      <c r="L51" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" t="s">
+        <v>18</v>
+      </c>
+      <c r="N51" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>